<commit_message>
docs(elaboracion 2/Estimación): agregar excel y documento de estimación
</commit_message>
<xml_diff>
--- a/Registro de tiempos por tarea - Kairos _ NexTech.xlsx
+++ b/Registro de tiempos por tarea - Kairos _ NexTech.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Fase Elaboración Iteración 2" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>Tarea</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Producto final</t>
   </si>
   <si>
-    <t>Tiempo total</t>
+    <t>Tiempo registrado</t>
   </si>
   <si>
     <t>Identificación y evaluación de riesgos</t>
@@ -61,36 +61,63 @@
     <t>Agustina Maldonado</t>
   </si>
   <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>01:00:00</t>
+  </si>
+  <si>
     <t>Redefinición de casos de uso</t>
   </si>
   <si>
     <t>gonzalo.ulloa99@gmail.com</t>
   </si>
   <si>
-    <t>Completado</t>
-  </si>
-  <si>
     <t>Modelo de Casos de Uso</t>
   </si>
   <si>
     <t>esstefaniamendez@gmail.com</t>
   </si>
   <si>
+    <t>26/9/2025</t>
+  </si>
+  <si>
+    <t>02:14:00</t>
+  </si>
+  <si>
+    <t>Valeria Centurion</t>
+  </si>
+  <si>
+    <t>02:00:00</t>
+  </si>
+  <si>
     <t>Estudio y análisis de Toggl Track API</t>
   </si>
   <si>
     <t>Capacitación</t>
   </si>
   <si>
+    <t>Sin comenzar</t>
+  </si>
+  <si>
     <t>Revisión de Modelo de Casos de Uso</t>
   </si>
   <si>
     <t>Validación y Verificación</t>
   </si>
   <si>
+    <t>00:20:00</t>
+  </si>
+  <si>
     <t>Estimación Fase Elaboración Iteración 2</t>
   </si>
   <si>
+    <t>30/9/2025</t>
+  </si>
+  <si>
+    <t>4:00:00</t>
+  </si>
+  <si>
     <t>Revisión de Estimación Fase Elaboración Iteración</t>
   </si>
   <si>
@@ -106,6 +133,12 @@
     <t>Diseño</t>
   </si>
   <si>
+    <t>Florencia Mendez</t>
+  </si>
+  <si>
+    <t>2:45:48</t>
+  </si>
+  <si>
     <t>Presentación 30/09</t>
   </si>
   <si>
@@ -118,6 +151,9 @@
     <t>Modelo De Datos (BD)</t>
   </si>
   <si>
+    <t>3/10/2025</t>
+  </si>
+  <si>
     <t>Aprobación Prototipo Funcional</t>
   </si>
   <si>
@@ -127,6 +163,9 @@
     <t>Documentación</t>
   </si>
   <si>
+    <t>7/10/2025</t>
+  </si>
+  <si>
     <t>Inicio Modelo de Diseño</t>
   </si>
   <si>
@@ -137,6 +176,9 @@
   </si>
   <si>
     <t>Codificación</t>
+  </si>
+  <si>
+    <t>10/10/2025</t>
   </si>
   <si>
     <t>Cierre Fase Elaboración - Iteración 2</t>
@@ -149,12 +191,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
     <numFmt numFmtId="165" formatCode="d/M/yyyy"/>
-    <numFmt numFmtId="166" formatCode="d/m"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -183,6 +224,18 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,49 +249,49 @@
     <border/>
     <border>
       <left style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </left>
       <right style="thin">
-        <color rgb="FF49564C"/>
+        <color rgb="FF535FC1"/>
       </right>
       <top style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF49564C"/>
+        <color rgb="FF535FC1"/>
       </left>
       <right style="thin">
-        <color rgb="FF49564C"/>
+        <color rgb="FF535FC1"/>
       </right>
       <top style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF49564C"/>
+        <color rgb="FF535FC1"/>
       </left>
       <right style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </right>
       <top style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
@@ -269,7 +322,7 @@
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
@@ -280,7 +333,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </left>
       <right style="thin">
         <color rgb="FFF6F8F9"/>
@@ -311,7 +364,7 @@
         <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </right>
       <top style="thin">
         <color rgb="FFF6F8F9"/>
@@ -322,7 +375,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
@@ -331,7 +384,7 @@
         <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
     <border>
@@ -345,7 +398,7 @@
         <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
     <border>
@@ -353,20 +406,20 @@
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </right>
       <top style="thin">
         <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF374139"/>
+        <color rgb="FF3E4791"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -376,8 +429,11 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -389,7 +445,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -397,8 +453,8 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -409,50 +465,57 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -466,14 +529,14 @@
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,8 +554,8 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF49564C"/>
-          <bgColor rgb="FF49564C"/>
+          <fgColor rgb="FF535FC1"/>
+          <bgColor rgb="FF535FC1"/>
         </patternFill>
       </fill>
       <border/>
@@ -519,7 +582,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Hoja 1-style">
+    <tableStyle count="3" pivot="0" name="Fase Elaboración Iteración 2-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -533,7 +596,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I24" displayName="Tareas_del_proyecto" name="Tareas_del_proyecto" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I26" displayName="Tareas_del_proyecto" name="Tareas_del_proyecto" id="1">
   <tableColumns count="9">
     <tableColumn name="Tarea" id="1"/>
     <tableColumn name="Categoría" id="2"/>
@@ -543,9 +606,9 @@
     <tableColumn name="Fecha de finalización" id="6"/>
     <tableColumn name="Fecha de Entrega" id="7"/>
     <tableColumn name="Producto final" id="8"/>
-    <tableColumn name="Tiempo total" id="9"/>
+    <tableColumn name="Tiempo registrado" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="Hoja 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Fase Elaboración Iteración 2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -759,11 +822,12 @@
     <col customWidth="1" min="1" max="1" width="31.63"/>
     <col customWidth="1" min="2" max="2" width="15.13"/>
     <col customWidth="1" min="3" max="3" width="18.75"/>
-    <col customWidth="1" min="4" max="4" width="15.13"/>
-    <col customWidth="1" min="5" max="6" width="20.13"/>
-    <col customWidth="1" min="7" max="7" width="21.63"/>
-    <col customWidth="1" min="8" max="8" width="22.63"/>
-    <col customWidth="1" min="9" max="9" width="18.13"/>
+    <col customWidth="1" min="4" max="4" width="16.13"/>
+    <col customWidth="1" min="5" max="5" width="11.63"/>
+    <col customWidth="1" min="6" max="6" width="13.88"/>
+    <col customWidth="1" min="7" max="7" width="12.75"/>
+    <col customWidth="1" hidden="1" min="8" max="8" width="22.63"/>
+    <col customWidth="1" min="9" max="9" width="15.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -779,59 +843,61 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>45923.0</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>45923.0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>12</v>
+      <c r="D3" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="15">
         <v>45923.0</v>
@@ -843,47 +909,49 @@
         <v>13</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="I3" s="18" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E4" s="8">
+        <v>45923.0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>45924.0</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="7">
-        <v>45923.0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>45924.0</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="19">
-        <v>0.020833333333333332</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>18</v>
+      <c r="C5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="E5" s="15">
         <v>45924.0</v>
@@ -891,430 +959,523 @@
       <c r="F5" s="15">
         <v>45926.0</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="22">
+        <v>45924.0</v>
+      </c>
+      <c r="F6" s="22">
         <v>45926.0</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="21">
-        <v>0.09305555555555556</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="G6" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="7">
+      <c r="H6" s="10"/>
+      <c r="I6" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="24">
         <v>45926.0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="24">
         <v>45927.0</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="G7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="22">
+        <v>45926.0</v>
+      </c>
+      <c r="F8" s="22">
+        <v>45926.0</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="15">
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="24">
+        <v>45928.0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>45928.0</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="22">
+        <v>45929.0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>45930.0</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="27" t="str">
+        <f>L7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="24">
         <v>45926.0</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F11" s="24">
         <v>45926.0</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="7">
-        <v>45928.0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>45928.0</v>
-      </c>
-      <c r="G8" s="25">
+      <c r="G11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="22">
+        <v>45926.0</v>
+      </c>
+      <c r="F12" s="22">
+        <v>45929.0</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="24">
+        <v>45929.0</v>
+      </c>
+      <c r="F13" s="24">
         <v>45930.0</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="15">
-        <v>45929.0</v>
-      </c>
-      <c r="F9" s="15">
+      <c r="G13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="22">
         <v>45930.0</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="24" t="s">
+      <c r="F14" s="22">
+        <v>45930.0</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="24">
+        <v>45930.0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>45901.0</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="7">
-        <v>45926.0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>45926.0</v>
-      </c>
-      <c r="G10" s="25">
-        <v>45926.0</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="22">
+        <v>45931.0</v>
+      </c>
+      <c r="F16" s="22">
+        <v>45931.0</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="24">
+        <v>45934.0</v>
+      </c>
+      <c r="F17" s="24">
+        <v>45934.0</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="22">
+        <v>45931.0</v>
+      </c>
+      <c r="F18" s="22">
+        <v>45933.0</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="24">
+        <v>45932.0</v>
+      </c>
+      <c r="F19" s="24">
+        <v>45932.0</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="22">
+        <v>45923.0</v>
+      </c>
+      <c r="F20" s="22">
+        <v>45937.0</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="24">
+        <v>45934.0</v>
+      </c>
+      <c r="F21" s="24">
+        <v>45936.0</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="22">
+        <v>45934.0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>45934.0</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="15">
-        <v>45926.0</v>
-      </c>
-      <c r="F11" s="15">
-        <v>45929.0</v>
-      </c>
-      <c r="G11" s="20">
-        <v>45930.0</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="7">
-        <v>45930.0</v>
-      </c>
-      <c r="F12" s="7">
-        <v>45930.0</v>
-      </c>
-      <c r="G12" s="25">
-        <v>45930.0</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="15">
-        <v>45930.0</v>
-      </c>
-      <c r="F13" s="15">
-        <v>45901.0</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="7">
-        <v>45931.0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>45931.0</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="15">
+      <c r="C23" s="17"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="24">
         <v>45934.0</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F23" s="24">
         <v>45934.0</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="7">
-        <v>45931.0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>45933.0</v>
-      </c>
-      <c r="G16" s="25">
-        <v>45933.0</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="15">
-        <v>45932.0</v>
-      </c>
-      <c r="F17" s="15">
-        <v>45932.0</v>
-      </c>
-      <c r="G17" s="20">
-        <v>45933.0</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="7">
-        <v>45923.0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>45937.0</v>
-      </c>
-      <c r="G18" s="25">
-        <v>45937.0</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="15">
-        <v>45934.0</v>
-      </c>
-      <c r="F19" s="15">
-        <v>45936.0</v>
-      </c>
-      <c r="G19" s="20">
-        <v>45937.0</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="7">
-        <v>45934.0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>45934.0</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="15">
-        <v>45934.0</v>
-      </c>
-      <c r="F21" s="15">
-        <v>45934.0</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="27">
+      <c r="G23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="22">
         <v>45935.0</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F24" s="22">
         <v>45935.0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="24">
         <v>45940.0</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="28">
+      <c r="F25" s="24">
         <v>45940.0</v>
       </c>
-      <c r="F23" s="28">
+      <c r="G25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37">
         <v>45940.0</v>
       </c>
-      <c r="G23" s="20">
+      <c r="F26" s="37">
         <v>45940.0</v>
       </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33">
-        <v>45940.0</v>
-      </c>
-      <c r="F24" s="33">
-        <v>45940.0</v>
-      </c>
-      <c r="G24" s="34">
-        <v>45940.0</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="35"/>
+      <c r="G26" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="39"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D24">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D26">
       <formula1>"Sin comenzar,En curso,Bloqueado,Completado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B24">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B26">
       <formula1>"Análisis,Documentación,Codificación,Validación y Verificación,Diseño,Otros,Capacitación"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:G24">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F26">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:I24">
-      <formula1>AND(ISNUMBER(I2),(NOT(OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D")))))</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A24"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A26 G2:G26 I2:I26"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
@@ -1322,10 +1483,15 @@
     <hyperlink r:id="rId3" ref="C4"/>
     <hyperlink r:id="rId4" ref="C5"/>
     <hyperlink r:id="rId5" ref="C6"/>
+    <hyperlink r:id="rId6" ref="C7"/>
+    <hyperlink r:id="rId7" ref="C8"/>
+    <hyperlink r:id="rId8" ref="C9"/>
+    <hyperlink r:id="rId9" ref="C12"/>
+    <hyperlink r:id="rId10" ref="C13"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs(Estimacion): Estimacion 03 Kairos
</commit_message>
<xml_diff>
--- a/Registro de tiempos por tarea - Kairos _ NexTech.xlsx
+++ b/Registro de tiempos por tarea - Kairos _ NexTech.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t>Tarea</t>
   </si>
@@ -115,22 +115,28 @@
     <t>30/9/2025</t>
   </si>
   <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>Revisión de Estimación Fase Elaboración Iteración</t>
+  </si>
+  <si>
+    <t>Presentación 26/09</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Primer Prototipo Funcional</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
     <t>4:00:00</t>
-  </si>
-  <si>
-    <t>Revisión de Estimación Fase Elaboración Iteración</t>
-  </si>
-  <si>
-    <t>Presentación 26/09</t>
-  </si>
-  <si>
-    <t>Otros</t>
-  </si>
-  <si>
-    <t>Primer Prototipo Funcional</t>
-  </si>
-  <si>
-    <t>Diseño</t>
   </si>
   <si>
     <t>Florencia Mendez</t>
@@ -195,7 +201,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm"/>
     <numFmt numFmtId="165" formatCode="d/M/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -230,12 +236,6 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -378,10 +378,10 @@
         <color rgb="FF3E4791"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF3E4791"/>
@@ -389,13 +389,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF3E4791"/>
@@ -403,13 +403,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
         <color rgb="FF3E4791"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF3E4791"/>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -502,19 +502,16 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -596,7 +593,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I26" displayName="Tareas_del_proyecto" name="Tareas_del_proyecto" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I27" displayName="Tareas_del_proyecto" name="Tareas_del_proyecto" id="1">
   <tableColumns count="9">
     <tableColumn name="Tarea" id="1"/>
     <tableColumn name="Categoría" id="2"/>
@@ -1059,7 +1056,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" s="24">
         <v>45928.0</v>
@@ -1077,27 +1074,29 @@
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E10" s="22">
         <v>45929.0</v>
       </c>
       <c r="F10" s="22">
-        <v>45930.0</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>13</v>
+        <v>45929.0</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="11" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="L10" s="27" t="str">
         <f>L7</f>
@@ -1109,20 +1108,20 @@
         <v>36</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E11" s="24">
-        <v>45926.0</v>
+        <v>45929.0</v>
       </c>
       <c r="F11" s="24">
-        <v>45926.0</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>22</v>
+        <v>45930.0</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="18" t="s">
@@ -1131,49 +1130,47 @@
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="C12" s="10"/>
       <c r="D12" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E12" s="22">
         <v>45926.0</v>
       </c>
       <c r="F12" s="22">
-        <v>45929.0</v>
+        <v>45926.0</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="11" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="28" t="s">
         <v>40</v>
       </c>
+      <c r="C13" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="D13" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E13" s="24">
+        <v>45926.0</v>
+      </c>
+      <c r="F13" s="24">
         <v>45929.0</v>
-      </c>
-      <c r="F13" s="24">
-        <v>45930.0</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>33</v>
@@ -1185,17 +1182,19 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="10"/>
       <c r="D14" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E14" s="22">
-        <v>45930.0</v>
+        <v>45929.0</v>
       </c>
       <c r="F14" s="22">
         <v>45930.0</v>
@@ -1205,15 +1204,15 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="11" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="13" t="s">
@@ -1223,10 +1222,10 @@
         <v>45930.0</v>
       </c>
       <c r="F15" s="24">
-        <v>45901.0</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>13</v>
+        <v>45930.0</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="18" t="s">
@@ -1235,160 +1234,164 @@
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="29"/>
+      <c r="D16" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="E16" s="22">
-        <v>45931.0</v>
+        <v>45930.0</v>
       </c>
       <c r="F16" s="22">
-        <v>45931.0</v>
+        <v>45901.0</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="10"/>
-      <c r="I16" s="30"/>
+      <c r="I16" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="17"/>
-      <c r="D17" s="31"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="24">
-        <v>45934.0</v>
+        <v>45931.0</v>
       </c>
       <c r="F17" s="24">
-        <v>45934.0</v>
+        <v>45931.0</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="17"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="29"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="22">
-        <v>45931.0</v>
+        <v>45934.0</v>
       </c>
       <c r="F18" s="22">
-        <v>45933.0</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>46</v>
+        <v>45934.0</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="30"/>
+      <c r="I18" s="31"/>
     </row>
     <row r="19">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="31"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="24">
-        <v>45932.0</v>
+        <v>45931.0</v>
       </c>
       <c r="F19" s="24">
-        <v>45932.0</v>
+        <v>45933.0</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H19" s="17"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="22">
+        <v>45932.0</v>
+      </c>
+      <c r="F20" s="22">
+        <v>45932.0</v>
+      </c>
+      <c r="G20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="22">
-        <v>45923.0</v>
-      </c>
-      <c r="F20" s="22">
-        <v>45937.0</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>50</v>
-      </c>
       <c r="H20" s="10"/>
-      <c r="I20" s="30"/>
+      <c r="I20" s="31"/>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="31"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="24">
-        <v>45934.0</v>
+        <v>45923.0</v>
       </c>
       <c r="F21" s="24">
-        <v>45936.0</v>
+        <v>45937.0</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H21" s="17"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="29"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="22">
         <v>45934.0</v>
       </c>
       <c r="F22" s="22">
-        <v>45934.0</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>13</v>
+        <v>45936.0</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="H22" s="10"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="31"/>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="31"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="24">
         <v>45934.0</v>
       </c>
@@ -1399,83 +1402,104 @@
         <v>13</v>
       </c>
       <c r="H23" s="17"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24">
       <c r="A24" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="22">
-        <v>45935.0</v>
+        <v>45934.0</v>
       </c>
       <c r="F24" s="22">
-        <v>45935.0</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>55</v>
+        <v>45934.0</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="H24" s="10"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="31"/>
     </row>
     <row r="25">
       <c r="A25" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="31"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="24">
+        <v>45935.0</v>
+      </c>
+      <c r="F25" s="24">
+        <v>45935.0</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="22">
         <v>45940.0</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F26" s="22">
         <v>45940.0</v>
       </c>
-      <c r="G25" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="32"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="33" t="s">
+      <c r="G26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37">
+      <c r="H26" s="10"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="36">
         <v>45940.0</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F27" s="36">
         <v>45940.0</v>
       </c>
-      <c r="G26" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="39"/>
+      <c r="G27" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="34"/>
+      <c r="I27" s="38"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D26">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D27">
       <formula1>"Sin comenzar,En curso,Bloqueado,Completado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B26">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B27">
       <formula1>"Análisis,Documentación,Codificación,Validación y Verificación,Diseño,Otros,Capacitación"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F26">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F27">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A26 G2:G26 I2:I26"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A27 G2:G27 I2:I27"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
@@ -1486,12 +1510,13 @@
     <hyperlink r:id="rId6" ref="C7"/>
     <hyperlink r:id="rId7" ref="C8"/>
     <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C12"/>
+    <hyperlink r:id="rId9" ref="C10"/>
     <hyperlink r:id="rId10" ref="C13"/>
+    <hyperlink r:id="rId11" ref="C14"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>